<commit_message>
Fixed reports problem in jupyter
Now chosen reports will be correctly added to the reports list in Jupyter main. Also text under papermill is not shown anymore when the notebook has been run successfully to make it a bit easier on the eye
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Adjusted default/specially chosen investment cost in jupyter
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Electrolyzer_PEM</t>
+          <t>PEM_Electrolyzer</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Methanol_Plant</t>
+          <t>Destilation_tower</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
reordering cells in the data prep
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
implement function to update investment cost set by user
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
test run and update of comments in the main file
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fix unlimited power flow for methanol reactor
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
bug fix of missing res values in investment_params info df
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Update for capacities = 100
Not yet removed the columns from input database as that will require major alterations to the code.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Update for in-/excluding grid
+ warning that at least one power source needs to be connected
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,70 +520,58 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>power_line_Wholesale_Kasso</t>
+          <t>pipeline_storage_hydrogen</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Power_line</t>
+          <t>Hydrogen_pipeline</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>pipeline_storage_hydrogen</t>
+          <t>pipeline_storage_e-methanol</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hydrogen_pipeline</t>
+          <t>Methanol_pipeline</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>pipeline_storage_e-methanol</t>
+          <t>pipeline_District_Heating</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Methanol_pipeline</t>
+          <t>Heat_pipeline</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>pipeline_District_Heating</t>
+          <t>Hydrogen_storage_Kasso</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Heat_pipeline</t>
+          <t>Hydrogen_storage</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hydrogen_storage_Kasso</t>
+          <t>E-Methanol_storage_Kasso</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
-        <is>
-          <t>Hydrogen_storage</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>E-Methanol_storage_Kasso</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
         <is>
           <t>Methanol_storage</t>
         </is>

</xml_diff>

<commit_message>
minor adjustment in data_prep_main
make the hint bigger to use the correct kernel for execution.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fix bug in map_parameters_by_similarity
function now returns only values of units that are part of the unit.
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
bug fixing and testing
investment parameter values are still having some bugs
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
add missing parameter for distillation tower
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
add further input files
only PV and sensitivities
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
add input files for further sensitivities
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
+++ b/Spine_Projects/01_input_data/02_input_prepared/methanol_object_mapping.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Object_Mapping" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>